<commit_message>
calculating pathline flux based on water balance
</commit_message>
<xml_diff>
--- a/research/check_effect_ncols_nlayers_pointparameter_distribution_SR.xlsx
+++ b/research/check_effect_ncols_nlayers_pointparameter_distribution_SR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sutra2_tool\sutra2\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBA3092-D274-4CEF-9623-5065CE10156C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2552CC8A-D7A5-4C7F-8DA6-F264D895E666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="5" xr2:uid="{F3AE1DE3-37C8-416A-B3FB-C4914D5D4B8E}"/>
+    <workbookView xWindow="28680" yWindow="-1995" windowWidth="29040" windowHeight="17640" firstSheet="4" activeTab="5" xr2:uid="{F3AE1DE3-37C8-416A-B3FB-C4914D5D4B8E}"/>
   </bookViews>
   <sheets>
     <sheet name="points" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="50">
   <si>
     <t>test_phreatic_defecation_withgravelpack</t>
   </si>
@@ -176,6 +176,21 @@
   </si>
   <si>
     <t>Conc vs radius</t>
+  </si>
+  <si>
+    <t>df_conc_cellflux based</t>
+  </si>
+  <si>
+    <t>Conc_diffuse</t>
+  </si>
+  <si>
+    <t>Conc_points</t>
+  </si>
+  <si>
+    <t>df_conc_points</t>
+  </si>
+  <si>
+    <t>df_conc_diffuse</t>
   </si>
 </sst>
 </file>
@@ -697,20 +712,117 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12496313479487263"/>
+          <c:y val="5.3112599852258011E-2"/>
+          <c:w val="0.83199398830332927"/>
+          <c:h val="0.72343581112292665"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>scenarios_diffuse_sensitivity!$AB$16</c:f>
+              <c:f>scenarios_diffuse_sensitivity!$AC$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>df_conc</c:v>
+                  <c:v>Conc_diffuse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scenarios_diffuse_sensitivity!$Y$17:$Y$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scenarios_diffuse_sensitivity!$AC$17:$AC$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>22.5338099981889</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38.967405928679099</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56.079779099237498</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69.083452704603602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.505617585429498</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37.599247231723098</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A368-4CAD-8C03-0BB0A8A9BC00}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>scenarios_diffuse_sensitivity!$AD$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Conc_points</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -729,7 +841,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>scenarios_diffuse_sensitivity!$X$17:$X$22</c:f>
+              <c:f>scenarios_diffuse_sensitivity!$Y$17:$Y$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -756,27 +868,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>scenarios_diffuse_sensitivity!$AB$17:$AB$22</c:f>
+              <c:f>scenarios_diffuse_sensitivity!$AD$17:$AD$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>22.5338099981889</c:v>
+                  <c:v>26.953481549250402</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.967405928679099</c:v>
+                  <c:v>40.514018835774202</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56.079779099237498</c:v>
+                  <c:v>53.989366503020499</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>69.083452704603602</c:v>
+                  <c:v>66.708492920955294</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57.505617585429498</c:v>
+                  <c:v>51.121952225615402</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.599247231723098</c:v>
+                  <c:v>31.682599794671599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1041,6 +1153,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2729,11 +2872,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>scenarios_diffuse_sensitivity!$M$1</c:f>
+              <c:f>scenarios_diffuse_sensitivity!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>df_conc</c:v>
+                  <c:v>Conc_points</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2779,27 +2922,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>scenarios_diffuse_sensitivity!$M$2:$M$7</c:f>
+              <c:f>scenarios_diffuse_sensitivity!$N$2:$N$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>25.5142715540156</c:v>
+                  <c:v>30.488602852813901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.912556563212497</c:v>
+                  <c:v>47.145948184568397</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58.495016730010299</c:v>
+                  <c:v>55.976172615030599</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65.105000000000004</c:v>
+                  <c:v>58.259164607314197</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68.970674784065494</c:v>
+                  <c:v>60.669777461330497</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>71.260437855413997</c:v>
+                  <c:v>59.074876438051099</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2808,6 +2951,93 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F5B9-4131-936A-A5C012B09DF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>scenarios_diffuse_sensitivity!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Conc_diffuse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scenarios_diffuse_sensitivity!$I$2:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scenarios_diffuse_sensitivity!$M$2:$M$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>25.5142715540156</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.912556563212497</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.495016730010299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.105000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68.970674784065494</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71.260437855413997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CFAD-45E8-94AF-64403C4C9E5A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3138,11 +3368,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>scenarios_diffuse_sensitivity!$S$1</c:f>
+              <c:f>scenarios_diffuse_sensitivity!$U$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>df_conc</c:v>
+                  <c:v>Conc_points</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3161,7 +3391,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>scenarios_diffuse_sensitivity!$P$2:$P$7</c:f>
+              <c:f>scenarios_diffuse_sensitivity!$Q$2:$Q$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3188,27 +3418,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>scenarios_diffuse_sensitivity!$S$2:$S$7</c:f>
+              <c:f>scenarios_diffuse_sensitivity!$U$2:$U$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>84.239617730598596</c:v>
+                  <c:v>73.530652211882</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68.079633351404894</c:v>
+                  <c:v>60.561798119740402</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.856107087789596</c:v>
+                  <c:v>58.112750469617403</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65.105000000000004</c:v>
+                  <c:v>58.259164607314197</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>65.377271664508001</c:v>
+                  <c:v>58.412875175862901</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>65.450543943517303</c:v>
+                  <c:v>58.497180231376703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3217,6 +3447,93 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F734-41DA-8DBF-46A519B18351}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>scenarios_diffuse_sensitivity!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Conc_diffuse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scenarios_diffuse_sensitivity!$Q$2:$Q$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scenarios_diffuse_sensitivity!$T$2:$T$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>84.239617730598596</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.079633351404894</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.856107087789596</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.105000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65.377271664508001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65.450543943517303</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-27A0-4089-BD85-0585DDB50321}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3473,6 +3790,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -3533,7 +3881,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12961927027933193"/>
+          <c:y val="5.5197123269755885E-2"/>
+          <c:w val="0.82573407209726235"/>
+          <c:h val="0.64233054344867047"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -3542,11 +3900,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>scenarios_diffuse_sensitivity!$M$9</c:f>
+              <c:f>scenarios_diffuse_sensitivity!$N$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>df_conc</c:v>
+                  <c:v>Conc_points</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3592,27 +3950,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>scenarios_diffuse_sensitivity!$M$10:$M$15</c:f>
+              <c:f>scenarios_diffuse_sensitivity!$N$10:$N$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>36.449204579620698</c:v>
+                  <c:v>30.1830444101038</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.798075477137701</c:v>
+                  <c:v>46.263802582230902</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65.105000000000004</c:v>
+                  <c:v>58.259164607314197</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>73.126591575894494</c:v>
+                  <c:v>66.069797313389998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>64.277107303678207</c:v>
+                  <c:v>57.714170952669498</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38.288895875584799</c:v>
+                  <c:v>33.126508638956103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3621,6 +3979,93 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-04D7-4BA8-A30D-27A0179CC2BE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>scenarios_diffuse_sensitivity!$M$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Conc_diffuse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scenarios_diffuse_sensitivity!$K$10:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scenarios_diffuse_sensitivity!$M$10:$M$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>36.449204579620698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.798075477137701</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65.105000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>73.126591575894494</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.277107303678207</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.288895875584799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4C17-402D-A72C-3A4BB2BBAF74}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3882,6 +4327,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -3942,7 +4418,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12496313479487263"/>
+          <c:y val="4.6067783285539794E-2"/>
+          <c:w val="0.83199398830332927"/>
+          <c:h val="0.67593480877447776"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -3951,11 +4437,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>scenarios_diffuse_sensitivity!$S$9</c:f>
+              <c:f>scenarios_diffuse_sensitivity!$U$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>df_conc</c:v>
+                  <c:v>Conc_points</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3974,7 +4460,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>scenarios_diffuse_sensitivity!$R$10:$R$14</c:f>
+              <c:f>scenarios_diffuse_sensitivity!$S$10:$S$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3998,24 +4484,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>scenarios_diffuse_sensitivity!$S$10:$S$14</c:f>
+              <c:f>scenarios_diffuse_sensitivity!$U$10:$U$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>59.300528170322302</c:v>
+                  <c:v>53.818476840777997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65.105000000000004</c:v>
+                  <c:v>58.259164607314197</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67.220388148015303</c:v>
+                  <c:v>59.950818811013697</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68.305143639711204</c:v>
+                  <c:v>60.662480888164602</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>69.746166130281097</c:v>
+                  <c:v>61.895986534738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4024,6 +4510,87 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5662-4D40-8AB5-536D400B8356}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>scenarios_diffuse_sensitivity!$T$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Conc_diffuse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scenarios_diffuse_sensitivity!$S$10:$S$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scenarios_diffuse_sensitivity!$T$10:$T$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>59.300528170322302</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.105000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.220388148015303</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.305143639711204</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>69.746166130281097</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CD1D-4ECC-9D82-6B0D00994D30}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4280,6 +4847,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -9888,16 +10486,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>777240</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>153520</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>178285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>479611</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>357579</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9960,16 +10558,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1169446</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>325195</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>62865</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>125506</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>37764</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>74071</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9996,16 +10594,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>172010</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>147470</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>476809</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>158676</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10073,16 +10671,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>121921</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>421006</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>110762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10111,16 +10709,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>316230</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>558710</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>75111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>541020</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>251188</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>88718</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10150,15 +10748,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:colOff>99059</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>408215</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10187,16 +10785,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>596537</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>145867</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>285205</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>11702</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10225,16 +10823,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>87086</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>130629</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>197848</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>99606</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>391886</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>97972</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>502648</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>72664</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12089,8 +12687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DE1333-C5E7-44C8-9B36-3E8B6A12E383}">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView topLeftCell="G4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G27" sqref="G2:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12120,6 +12718,9 @@
       <c r="F1" t="s">
         <v>40</v>
       </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
       <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
@@ -12170,6 +12771,9 @@
       <c r="F2">
         <v>8.1099384933809109</v>
       </c>
+      <c r="G2">
+        <v>58.259164607314197</v>
+      </c>
       <c r="I2">
         <v>5</v>
       </c>
@@ -12220,6 +12824,9 @@
       <c r="F3">
         <v>4.6784848647522796</v>
       </c>
+      <c r="G3">
+        <v>30.488602852813901</v>
+      </c>
       <c r="I3">
         <v>10</v>
       </c>
@@ -12270,6 +12877,9 @@
       <c r="F4">
         <v>6.6720264941045899</v>
       </c>
+      <c r="G4">
+        <v>47.145948184568397</v>
+      </c>
       <c r="I4">
         <v>20</v>
       </c>
@@ -12320,6 +12930,9 @@
       <c r="F5">
         <v>7.6056669261403496</v>
       </c>
+      <c r="G5">
+        <v>55.976172615030599</v>
+      </c>
       <c r="I5">
         <v>40</v>
       </c>
@@ -12370,6 +12983,9 @@
       <c r="F6">
         <v>8.4608472248610198</v>
       </c>
+      <c r="G6">
+        <v>60.669777461330497</v>
+      </c>
       <c r="I6">
         <v>80</v>
       </c>
@@ -12420,6 +13036,9 @@
       <c r="F7">
         <v>8.6548337929535908</v>
       </c>
+      <c r="G7">
+        <v>59.074876438051099</v>
+      </c>
       <c r="I7">
         <v>160</v>
       </c>
@@ -12470,6 +13089,9 @@
       <c r="F8">
         <v>10.1114692363312</v>
       </c>
+      <c r="G8">
+        <v>73.530652211882</v>
+      </c>
     </row>
     <row r="9" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -12490,6 +13112,9 @@
       <c r="F9">
         <v>8.4253175726504494</v>
       </c>
+      <c r="G9">
+        <v>60.561798119740402</v>
+      </c>
       <c r="I9" s="7" t="s">
         <v>1</v>
       </c>
@@ -12540,6 +13165,9 @@
       <c r="F10">
         <v>8.0796448219710495</v>
       </c>
+      <c r="G10">
+        <v>58.112750469617403</v>
+      </c>
       <c r="I10">
         <v>40</v>
       </c>
@@ -12589,6 +13217,9 @@
       </c>
       <c r="F11">
         <v>8.1387009018225402</v>
+      </c>
+      <c r="G11">
+        <v>58.412875175862901</v>
       </c>
       <c r="I11">
         <v>40</v>
@@ -12640,6 +13271,9 @@
       <c r="F12">
         <v>8.1468615367858206</v>
       </c>
+      <c r="G12">
+        <v>58.497180231376703</v>
+      </c>
       <c r="I12">
         <v>40</v>
       </c>
@@ -12690,6 +13324,9 @@
       <c r="F13">
         <v>5.7686623600420104</v>
       </c>
+      <c r="G13">
+        <v>30.1830444101038</v>
+      </c>
       <c r="I13">
         <v>40</v>
       </c>
@@ -12740,6 +13377,9 @@
       <c r="F14">
         <v>7.1744752559169402</v>
       </c>
+      <c r="G14">
+        <v>46.263802582230902</v>
+      </c>
       <c r="I14">
         <v>40</v>
       </c>
@@ -12790,6 +13430,9 @@
       <c r="F15">
         <v>8.6419753815900506</v>
       </c>
+      <c r="G15">
+        <v>66.069797313389998</v>
+      </c>
       <c r="I15">
         <v>40</v>
       </c>
@@ -12825,6 +13468,9 @@
       <c r="F16">
         <v>8.0332178397855198</v>
       </c>
+      <c r="G16">
+        <v>57.714170952669498</v>
+      </c>
       <c r="W16" s="7" t="s">
         <v>1</v>
       </c>
@@ -12860,6 +13506,9 @@
       <c r="F17">
         <v>8.6786343450227701</v>
       </c>
+      <c r="G17">
+        <v>33.126508638956103</v>
+      </c>
       <c r="W17">
         <v>5</v>
       </c>
@@ -12895,6 +13544,9 @@
       <c r="F18">
         <v>7.4847732068583799</v>
       </c>
+      <c r="G18">
+        <v>53.818476840777997</v>
+      </c>
       <c r="W18">
         <v>10</v>
       </c>
@@ -12930,6 +13582,9 @@
       <c r="F19">
         <v>8.3404924524105102</v>
       </c>
+      <c r="G19">
+        <v>59.950818811013697</v>
+      </c>
       <c r="W19">
         <v>15</v>
       </c>
@@ -12965,6 +13620,9 @@
       <c r="F20">
         <v>8.4546560227959393</v>
       </c>
+      <c r="G20">
+        <v>60.662480888164602</v>
+      </c>
       <c r="W20">
         <v>20</v>
       </c>
@@ -13000,6 +13658,9 @@
       <c r="F21">
         <v>8.6091989579084398</v>
       </c>
+      <c r="G21">
+        <v>61.895986534738</v>
+      </c>
       <c r="W21">
         <v>40</v>
       </c>
@@ -13035,6 +13696,9 @@
       <c r="F22">
         <v>4.3074324846023604</v>
       </c>
+      <c r="G22">
+        <v>26.953481549250402</v>
+      </c>
       <c r="W22">
         <v>80</v>
       </c>
@@ -13070,6 +13734,9 @@
       <c r="F23">
         <v>5.9921622913398203</v>
       </c>
+      <c r="G23">
+        <v>40.514018835774202</v>
+      </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -13090,6 +13757,9 @@
       <c r="F24">
         <v>7.4943840190021298</v>
       </c>
+      <c r="G24">
+        <v>53.989366503020499</v>
+      </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -13110,6 +13780,9 @@
       <c r="F25">
         <v>8.4790016629139693</v>
       </c>
+      <c r="G25">
+        <v>66.708492920955294</v>
+      </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -13130,6 +13803,9 @@
       <c r="F26">
         <v>9.1496005794780597</v>
       </c>
+      <c r="G26">
+        <v>51.121952225615402</v>
+      </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27">
@@ -13149,6 +13825,9 @@
       </c>
       <c r="F27">
         <v>10.181562281466899</v>
+      </c>
+      <c r="G27">
+        <v>31.682599794671599</v>
       </c>
     </row>
   </sheetData>
@@ -13160,10 +13839,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76426CD9-C6E8-473D-ACEA-52258FA2CC17}">
-  <dimension ref="A1:AB27"/>
+  <dimension ref="A1:AD27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13172,9 +13851,11 @@
     <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -13191,7 +13872,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>1</v>
@@ -13206,25 +13890,32 @@
         <v>4</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="7" t="s">
-        <v>40</v>
+      <c r="T1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -13243,6 +13934,9 @@
       <c r="F2">
         <v>65.105000000000004</v>
       </c>
+      <c r="G2">
+        <v>58.259164607314197</v>
+      </c>
       <c r="I2">
         <v>5</v>
       </c>
@@ -13258,23 +13952,29 @@
       <c r="M2">
         <v>25.5142715540156</v>
       </c>
-      <c r="O2">
-        <v>40</v>
+      <c r="N2">
+        <v>30.488602852813901</v>
       </c>
       <c r="P2">
+        <v>40</v>
+      </c>
+      <c r="Q2">
         <v>5</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>15</v>
       </c>
-      <c r="R2">
-        <v>10</v>
-      </c>
       <c r="S2">
+        <v>10</v>
+      </c>
+      <c r="T2">
         <v>84.239617730598596</v>
       </c>
+      <c r="U2">
+        <v>73.530652211882</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -13293,6 +13993,9 @@
       <c r="F3">
         <v>25.5142715540156</v>
       </c>
+      <c r="G3">
+        <v>30.488602852813901</v>
+      </c>
       <c r="I3">
         <v>10</v>
       </c>
@@ -13308,23 +14011,29 @@
       <c r="M3">
         <v>45.912556563212497</v>
       </c>
-      <c r="O3">
-        <v>40</v>
+      <c r="N3">
+        <v>47.145948184568397</v>
       </c>
       <c r="P3">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="Q3">
+        <v>10</v>
+      </c>
+      <c r="R3">
         <v>15</v>
       </c>
-      <c r="R3">
-        <v>10</v>
-      </c>
       <c r="S3">
+        <v>10</v>
+      </c>
+      <c r="T3">
         <v>68.079633351404894</v>
       </c>
+      <c r="U3">
+        <v>60.561798119740402</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -13343,6 +14052,9 @@
       <c r="F4">
         <v>45.912556563212497</v>
       </c>
+      <c r="G4">
+        <v>47.145948184568397</v>
+      </c>
       <c r="I4">
         <v>20</v>
       </c>
@@ -13358,23 +14070,29 @@
       <c r="M4">
         <v>58.495016730010299</v>
       </c>
-      <c r="O4">
-        <v>40</v>
+      <c r="N4">
+        <v>55.976172615030599</v>
       </c>
       <c r="P4">
+        <v>40</v>
+      </c>
+      <c r="Q4">
         <v>20</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>15</v>
       </c>
-      <c r="R4">
-        <v>10</v>
-      </c>
       <c r="S4">
+        <v>10</v>
+      </c>
+      <c r="T4">
         <v>64.856107087789596</v>
       </c>
+      <c r="U4">
+        <v>58.112750469617403</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -13393,6 +14111,9 @@
       <c r="F5">
         <v>58.495016730010299</v>
       </c>
+      <c r="G5">
+        <v>55.976172615030599</v>
+      </c>
       <c r="I5">
         <v>40</v>
       </c>
@@ -13408,23 +14129,29 @@
       <c r="M5">
         <v>65.105000000000004</v>
       </c>
-      <c r="O5">
-        <v>40</v>
+      <c r="N5">
+        <v>58.259164607314197</v>
       </c>
       <c r="P5">
         <v>40</v>
       </c>
       <c r="Q5">
+        <v>40</v>
+      </c>
+      <c r="R5">
         <v>15</v>
       </c>
-      <c r="R5">
-        <v>10</v>
-      </c>
       <c r="S5">
+        <v>10</v>
+      </c>
+      <c r="T5">
         <v>65.105000000000004</v>
       </c>
+      <c r="U5">
+        <v>58.259164607314197</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -13443,6 +14170,9 @@
       <c r="F6">
         <v>68.970674784065494</v>
       </c>
+      <c r="G6">
+        <v>60.669777461330497</v>
+      </c>
       <c r="I6">
         <v>80</v>
       </c>
@@ -13458,23 +14188,29 @@
       <c r="M6">
         <v>68.970674784065494</v>
       </c>
-      <c r="O6">
-        <v>40</v>
+      <c r="N6">
+        <v>60.669777461330497</v>
       </c>
       <c r="P6">
+        <v>40</v>
+      </c>
+      <c r="Q6">
         <v>80</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>15</v>
       </c>
-      <c r="R6">
-        <v>10</v>
-      </c>
       <c r="S6">
+        <v>10</v>
+      </c>
+      <c r="T6">
         <v>65.377271664508001</v>
       </c>
+      <c r="U6">
+        <v>58.412875175862901</v>
+      </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -13493,6 +14229,9 @@
       <c r="F7">
         <v>71.260437855413997</v>
       </c>
+      <c r="G7">
+        <v>59.074876438051099</v>
+      </c>
       <c r="I7">
         <v>160</v>
       </c>
@@ -13508,23 +14247,29 @@
       <c r="M7">
         <v>71.260437855413997</v>
       </c>
-      <c r="O7">
-        <v>40</v>
+      <c r="N7">
+        <v>59.074876438051099</v>
       </c>
       <c r="P7">
+        <v>40</v>
+      </c>
+      <c r="Q7">
         <v>160</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>15</v>
       </c>
-      <c r="R7">
-        <v>10</v>
-      </c>
       <c r="S7">
+        <v>10</v>
+      </c>
+      <c r="T7">
         <v>65.450543943517303</v>
       </c>
+      <c r="U7">
+        <v>58.497180231376703</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -13543,8 +14288,11 @@
       <c r="F8">
         <v>84.239617730598596</v>
       </c>
+      <c r="G8">
+        <v>73.530652211882</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -13563,6 +14311,9 @@
       <c r="F9">
         <v>68.079633351404894</v>
       </c>
+      <c r="G9">
+        <v>60.561798119740402</v>
+      </c>
       <c r="I9" s="7" t="s">
         <v>1</v>
       </c>
@@ -13576,25 +14327,32 @@
         <v>4</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="O9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="P9" s="7" t="s">
+      <c r="Q9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="Q9" s="7" t="s">
+      <c r="R9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R9" s="6" t="s">
+      <c r="S9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="S9" s="7" t="s">
-        <v>40</v>
+      <c r="T9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U9" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -13613,6 +14371,9 @@
       <c r="F10">
         <v>64.856107087789596</v>
       </c>
+      <c r="G10">
+        <v>58.112750469617403</v>
+      </c>
       <c r="I10">
         <v>40</v>
       </c>
@@ -13628,23 +14389,29 @@
       <c r="M10">
         <v>36.449204579620698</v>
       </c>
-      <c r="O10">
-        <v>40</v>
+      <c r="N10">
+        <v>30.1830444101038</v>
       </c>
       <c r="P10">
         <v>40</v>
       </c>
       <c r="Q10">
+        <v>40</v>
+      </c>
+      <c r="R10">
         <v>15</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>5</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>59.300528170322302</v>
       </c>
+      <c r="U10">
+        <v>53.818476840777997</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -13663,6 +14430,9 @@
       <c r="F11">
         <v>65.377271664508001</v>
       </c>
+      <c r="G11">
+        <v>58.412875175862901</v>
+      </c>
       <c r="I11">
         <v>40</v>
       </c>
@@ -13678,23 +14448,29 @@
       <c r="M11">
         <v>52.798075477137701</v>
       </c>
-      <c r="O11">
-        <v>40</v>
+      <c r="N11">
+        <v>46.263802582230902</v>
       </c>
       <c r="P11">
         <v>40</v>
       </c>
       <c r="Q11">
+        <v>40</v>
+      </c>
+      <c r="R11">
         <v>15</v>
       </c>
-      <c r="R11">
-        <v>10</v>
-      </c>
       <c r="S11">
+        <v>10</v>
+      </c>
+      <c r="T11">
         <v>65.105000000000004</v>
       </c>
+      <c r="U11">
+        <v>58.259164607314197</v>
+      </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -13713,6 +14489,9 @@
       <c r="F12">
         <v>65.450543943517303</v>
       </c>
+      <c r="G12">
+        <v>58.497180231376703</v>
+      </c>
       <c r="I12">
         <v>40</v>
       </c>
@@ -13728,23 +14507,29 @@
       <c r="M12">
         <v>65.105000000000004</v>
       </c>
-      <c r="O12">
-        <v>40</v>
+      <c r="N12">
+        <v>58.259164607314197</v>
       </c>
       <c r="P12">
         <v>40</v>
       </c>
       <c r="Q12">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="R12">
         <v>15</v>
       </c>
       <c r="S12">
+        <v>15</v>
+      </c>
+      <c r="T12">
         <v>67.220388148015303</v>
       </c>
+      <c r="U12">
+        <v>59.950818811013697</v>
+      </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -13763,6 +14548,9 @@
       <c r="F13">
         <v>36.449204579620698</v>
       </c>
+      <c r="G13">
+        <v>30.1830444101038</v>
+      </c>
       <c r="I13">
         <v>40</v>
       </c>
@@ -13778,23 +14566,29 @@
       <c r="M13">
         <v>73.126591575894494</v>
       </c>
-      <c r="O13">
-        <v>40</v>
+      <c r="N13">
+        <v>66.069797313389998</v>
       </c>
       <c r="P13">
         <v>40</v>
       </c>
       <c r="Q13">
+        <v>40</v>
+      </c>
+      <c r="R13">
         <v>15</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>20</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>68.305143639711204</v>
       </c>
+      <c r="U13">
+        <v>60.662480888164602</v>
+      </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -13813,6 +14607,9 @@
       <c r="F14">
         <v>52.798075477137701</v>
       </c>
+      <c r="G14">
+        <v>46.263802582230902</v>
+      </c>
       <c r="I14">
         <v>40</v>
       </c>
@@ -13828,23 +14625,29 @@
       <c r="M14">
         <v>64.277107303678207</v>
       </c>
-      <c r="O14">
-        <v>40</v>
+      <c r="N14">
+        <v>57.714170952669498</v>
       </c>
       <c r="P14">
         <v>40</v>
       </c>
       <c r="Q14">
+        <v>40</v>
+      </c>
+      <c r="R14">
         <v>15</v>
       </c>
-      <c r="R14">
-        <v>40</v>
-      </c>
       <c r="S14">
+        <v>40</v>
+      </c>
+      <c r="T14">
         <v>69.746166130281097</v>
       </c>
+      <c r="U14">
+        <v>61.895986534738</v>
+      </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -13863,6 +14666,9 @@
       <c r="F15">
         <v>73.126591575894494</v>
       </c>
+      <c r="G15">
+        <v>66.069797313389998</v>
+      </c>
       <c r="I15">
         <v>40</v>
       </c>
@@ -13878,8 +14684,11 @@
       <c r="M15">
         <v>38.288895875584799</v>
       </c>
+      <c r="N15">
+        <v>33.126508638956103</v>
+      </c>
     </row>
-    <row r="16" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -13898,23 +14707,29 @@
       <c r="F16">
         <v>64.277107303678207</v>
       </c>
-      <c r="X16" s="7" t="s">
+      <c r="G16">
+        <v>57.714170952669498</v>
+      </c>
+      <c r="Y16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Y16" s="7" t="s">
+      <c r="Z16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="Z16" s="6" t="s">
+      <c r="AA16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="AA16" s="7" t="s">
+      <c r="AB16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AB16" s="7" t="s">
-        <v>40</v>
+      <c r="AC16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD16" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -13933,8 +14748,8 @@
       <c r="F17">
         <v>38.288895875584799</v>
       </c>
-      <c r="X17">
-        <v>5</v>
+      <c r="G17">
+        <v>33.126508638956103</v>
       </c>
       <c r="Y17">
         <v>5</v>
@@ -13946,10 +14761,16 @@
         <v>5</v>
       </c>
       <c r="AB17">
+        <v>5</v>
+      </c>
+      <c r="AC17">
         <v>22.5338099981889</v>
       </c>
+      <c r="AD17">
+        <v>26.953481549250402</v>
+      </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -13968,8 +14789,8 @@
       <c r="F18">
         <v>59.300528170322302</v>
       </c>
-      <c r="X18">
-        <v>10</v>
+      <c r="G18">
+        <v>53.818476840777997</v>
       </c>
       <c r="Y18">
         <v>10</v>
@@ -13981,10 +14802,16 @@
         <v>10</v>
       </c>
       <c r="AB18">
+        <v>10</v>
+      </c>
+      <c r="AC18">
         <v>38.967405928679099</v>
       </c>
+      <c r="AD18">
+        <v>40.514018835774202</v>
+      </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -14003,8 +14830,8 @@
       <c r="F19">
         <v>67.220388148015303</v>
       </c>
-      <c r="X19">
-        <v>15</v>
+      <c r="G19">
+        <v>59.950818811013697</v>
       </c>
       <c r="Y19">
         <v>15</v>
@@ -14016,10 +14843,16 @@
         <v>15</v>
       </c>
       <c r="AB19">
+        <v>15</v>
+      </c>
+      <c r="AC19">
         <v>56.079779099237498</v>
       </c>
+      <c r="AD19">
+        <v>53.989366503020499</v>
+      </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -14038,8 +14871,8 @@
       <c r="F20">
         <v>68.305143639711204</v>
       </c>
-      <c r="X20">
-        <v>20</v>
+      <c r="G20">
+        <v>60.662480888164602</v>
       </c>
       <c r="Y20">
         <v>20</v>
@@ -14051,10 +14884,16 @@
         <v>20</v>
       </c>
       <c r="AB20">
+        <v>20</v>
+      </c>
+      <c r="AC20">
         <v>69.083452704603602</v>
       </c>
+      <c r="AD20">
+        <v>66.708492920955294</v>
+      </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -14073,8 +14912,8 @@
       <c r="F21">
         <v>69.746166130281097</v>
       </c>
-      <c r="X21">
-        <v>40</v>
+      <c r="G21">
+        <v>61.895986534738</v>
       </c>
       <c r="Y21">
         <v>40</v>
@@ -14086,10 +14925,16 @@
         <v>40</v>
       </c>
       <c r="AB21">
+        <v>40</v>
+      </c>
+      <c r="AC21">
         <v>57.505617585429498</v>
       </c>
+      <c r="AD21">
+        <v>51.121952225615402</v>
+      </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -14108,8 +14953,8 @@
       <c r="F22">
         <v>22.5338099981889</v>
       </c>
-      <c r="X22">
-        <v>80</v>
+      <c r="G22">
+        <v>26.953481549250402</v>
       </c>
       <c r="Y22">
         <v>80</v>
@@ -14121,10 +14966,16 @@
         <v>80</v>
       </c>
       <c r="AB22">
+        <v>80</v>
+      </c>
+      <c r="AC22">
         <v>37.599247231723098</v>
       </c>
+      <c r="AD22">
+        <v>31.682599794671599</v>
+      </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -14143,8 +14994,11 @@
       <c r="F23">
         <v>38.967405928679099</v>
       </c>
+      <c r="G23">
+        <v>40.514018835774202</v>
+      </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -14163,8 +15017,11 @@
       <c r="F24">
         <v>56.079779099237498</v>
       </c>
+      <c r="G24">
+        <v>53.989366503020499</v>
+      </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -14183,8 +15040,11 @@
       <c r="F25">
         <v>69.083452704603602</v>
       </c>
+      <c r="G25">
+        <v>66.708492920955294</v>
+      </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -14203,8 +15063,11 @@
       <c r="F26">
         <v>57.505617585429498</v>
       </c>
+      <c r="G26">
+        <v>51.121952225615402</v>
+      </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -14222,6 +15085,9 @@
       </c>
       <c r="F27">
         <v>37.599247231723098</v>
+      </c>
+      <c r="G27">
+        <v>31.682599794671599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>